<commit_message>
Incorporated OPs consolidation in the script
</commit_message>
<xml_diff>
--- a/utils/config/ReferenceLists/New_OPS_not_in_EMS.xlsx
+++ b/utils/config/ReferenceLists/New_OPS_not_in_EMS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://bcgov-my.sharepoint.com/personal/sahil_bhandari_gov_bc_ca/Documents/teamdocs/GitHub/aqs-api/utils/config/ReferenceLists/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="121" documentId="8_{14914D35-8641-4F30-AE69-5AD2BBC1D42C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C0FDEEF-FE2E-4CEE-BB67-9A1A5524470B}"/>
+  <xr:revisionPtr revIDLastSave="124" documentId="8_{14914D35-8641-4F30-AE69-5AD2BBC1D42C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7CE7FDB9-5F6A-4164-BFAD-A7CD9909430A}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3030" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{1458A00D-CA65-4CF2-9307-1B9709084815}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{1458A00D-CA65-4CF2-9307-1B9709084815}"/>
   </bookViews>
   <sheets>
     <sheet name="OPs_new" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="116">
   <si>
     <t>Net Mesh Size (len.)</t>
   </si>
@@ -767,422 +767,428 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{232F1D4C-D575-4EB0-94BA-0D66318AA45B}">
-  <dimension ref="A1:AE14"/>
+  <dimension ref="A1:AF14"/>
   <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="AA14" sqref="AA14"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="T14" sqref="T14:U14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.26953125" customWidth="1"/>
-    <col min="2" max="2" width="80.1796875" customWidth="1"/>
-    <col min="3" max="3" width="41" customWidth="1"/>
-    <col min="4" max="4" width="24.1796875" customWidth="1"/>
-    <col min="5" max="5" width="22.26953125" customWidth="1"/>
-    <col min="13" max="13" width="26.7265625" customWidth="1"/>
-    <col min="14" max="14" width="25" customWidth="1"/>
-    <col min="15" max="15" width="17.54296875" customWidth="1"/>
-    <col min="19" max="19" width="20" customWidth="1"/>
-    <col min="20" max="20" width="31.26953125" customWidth="1"/>
-    <col min="21" max="22" width="28.26953125" customWidth="1"/>
-    <col min="23" max="23" width="23.54296875" customWidth="1"/>
-    <col min="24" max="24" width="31.54296875" customWidth="1"/>
-    <col min="25" max="26" width="19.1796875" customWidth="1"/>
-    <col min="27" max="27" width="64.54296875" customWidth="1"/>
-    <col min="28" max="29" width="40.7265625" customWidth="1"/>
-    <col min="30" max="30" width="31.81640625" customWidth="1"/>
-    <col min="31" max="31" width="25.81640625" customWidth="1"/>
+    <col min="1" max="1" width="31.54296875" customWidth="1"/>
+    <col min="2" max="2" width="35.26953125" customWidth="1"/>
+    <col min="3" max="3" width="80.1796875" customWidth="1"/>
+    <col min="4" max="4" width="41" customWidth="1"/>
+    <col min="5" max="5" width="24.1796875" customWidth="1"/>
+    <col min="6" max="6" width="22.26953125" customWidth="1"/>
+    <col min="14" max="14" width="26.7265625" customWidth="1"/>
+    <col min="15" max="15" width="25" customWidth="1"/>
+    <col min="16" max="16" width="17.54296875" customWidth="1"/>
+    <col min="20" max="20" width="20" customWidth="1"/>
+    <col min="21" max="21" width="31.26953125" customWidth="1"/>
+    <col min="22" max="23" width="28.26953125" customWidth="1"/>
+    <col min="24" max="24" width="23.54296875" customWidth="1"/>
+    <col min="26" max="27" width="19.1796875" customWidth="1"/>
+    <col min="28" max="28" width="64.54296875" customWidth="1"/>
+    <col min="29" max="30" width="40.7265625" customWidth="1"/>
+    <col min="31" max="31" width="31.81640625" customWidth="1"/>
+    <col min="32" max="32" width="25.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" s="1" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="X1" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="S2" t="s">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" t="s">
         <v>4</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>69</v>
       </c>
-      <c r="X2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>1</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>3</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>2</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="S3" t="s">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="T3" t="s">
         <v>4</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>7</v>
       </c>
-      <c r="X3" t="s">
-        <v>5</v>
-      </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>6</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>3</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>2</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AF3" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="S4" t="s">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>8</v>
+      </c>
+      <c r="T4" t="s">
         <v>4</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>10</v>
       </c>
-      <c r="X4" t="s">
-        <v>8</v>
-      </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
         <v>9</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
         <v>3</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AD4" t="s">
         <v>2</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AF4" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="S5" t="s">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>110</v>
+      </c>
+      <c r="T5" t="s">
         <v>13</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>111</v>
       </c>
-      <c r="X5" t="s">
-        <v>110</v>
-      </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>112</v>
       </c>
-      <c r="AB5" t="s">
+      <c r="AC5" t="s">
         <v>3</v>
       </c>
-      <c r="AC5" t="s">
+      <c r="AD5" t="s">
         <v>2</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AF5" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="S6" t="s">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="T6" t="s">
         <v>13</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>14</v>
       </c>
-      <c r="X6" t="s">
-        <v>11</v>
-      </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>12</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AC6" t="s">
         <v>3</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AD6" t="s">
         <v>2</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AF6" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
         <v>19</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>17</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>18</v>
       </c>
-      <c r="X7" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA7" t="s">
+      <c r="AB7" t="s">
         <v>16</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AC7" t="s">
         <v>3</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AD7" t="s">
         <v>2</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AF7" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>106</v>
+      </c>
+      <c r="B8" t="s">
         <v>21</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>4</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
         <v>7</v>
       </c>
-      <c r="X8" t="s">
-        <v>106</v>
-      </c>
-      <c r="AA8" t="s">
+      <c r="AB8" t="s">
         <v>20</v>
       </c>
-      <c r="AB8" t="s">
+      <c r="AC8" t="s">
         <v>3</v>
       </c>
-      <c r="AC8" t="s">
+      <c r="AD8" t="s">
         <v>2</v>
       </c>
-      <c r="AE8" t="s">
+      <c r="AF8" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
         <v>26</v>
       </c>
-      <c r="S9" t="s">
+      <c r="T9" t="s">
         <v>24</v>
       </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
         <v>25</v>
       </c>
-      <c r="X9" t="s">
-        <v>22</v>
-      </c>
-      <c r="AA9" t="s">
+      <c r="AB9" t="s">
         <v>23</v>
       </c>
-      <c r="AB9" t="s">
+      <c r="AC9" t="s">
         <v>3</v>
       </c>
-      <c r="AC9" t="s">
+      <c r="AD9" t="s">
         <v>2</v>
       </c>
-      <c r="AE9" t="s">
+      <c r="AF9" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>27</v>
+      </c>
+      <c r="B10" t="s">
         <v>29</v>
       </c>
-      <c r="X10" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA10" t="s">
+      <c r="AB10" t="s">
         <v>28</v>
       </c>
-      <c r="AC10" t="s">
+      <c r="AD10" t="s">
         <v>70</v>
       </c>
-      <c r="AE10" t="s">
+      <c r="AF10" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B11" t="s">
         <v>32</v>
       </c>
-      <c r="X11" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA11" t="s">
+      <c r="AB11" t="s">
         <v>31</v>
       </c>
-      <c r="AC11" t="s">
+      <c r="AD11" t="s">
         <v>70</v>
       </c>
-      <c r="AE11" t="s">
+      <c r="AF11" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>107</v>
+      </c>
+      <c r="B12" t="s">
         <v>34</v>
       </c>
-      <c r="S12" t="s">
+      <c r="T12" t="s">
         <v>4</v>
       </c>
-      <c r="T12" t="s">
+      <c r="U12" t="s">
         <v>69</v>
       </c>
-      <c r="X12" t="s">
-        <v>107</v>
-      </c>
-      <c r="AA12" t="s">
+      <c r="AB12" t="s">
         <v>33</v>
       </c>
-      <c r="AB12" t="s">
+      <c r="AC12" t="s">
         <v>3</v>
       </c>
-      <c r="AC12" t="s">
+      <c r="AD12" t="s">
         <v>2</v>
       </c>
-      <c r="AE12" t="s">
+      <c r="AF12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" t="s">
         <v>37</v>
       </c>
-      <c r="S13" t="s">
+      <c r="T13" t="s">
         <v>13</v>
       </c>
-      <c r="T13" t="s">
+      <c r="U13" t="s">
         <v>14</v>
       </c>
-      <c r="X13" t="s">
-        <v>35</v>
-      </c>
-      <c r="AA13" t="s">
+      <c r="AB13" t="s">
         <v>36</v>
       </c>
-      <c r="AB13" t="s">
+      <c r="AC13" t="s">
         <v>3</v>
       </c>
-      <c r="AC13" t="s">
+      <c r="AD13" t="s">
         <v>2</v>
       </c>
-      <c r="AE13" t="s">
+      <c r="AF13" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.35">
-      <c r="X14" t="s">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>113</v>
       </c>
-      <c r="AA14" t="s">
+      <c r="T14" t="s">
+        <v>13</v>
+      </c>
+      <c r="U14" t="s">
+        <v>14</v>
+      </c>
+      <c r="AB14" t="s">
         <v>114</v>
       </c>
-      <c r="AB14" t="s">
+      <c r="AC14" t="s">
         <v>3</v>
       </c>
-      <c r="AC14" t="s">
+      <c r="AD14" t="s">
         <v>2</v>
       </c>
-      <c r="AE14" t="s">
+      <c r="AF14" t="s">
         <v>115</v>
       </c>
     </row>
@@ -1195,7 +1201,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF183198-A4D3-4FFC-820E-9331077794FA}">
   <dimension ref="A1:B34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>

</xml_diff>